<commit_message>
implemented scraping from bestbuy, microcenter
</commit_message>
<xml_diff>
--- a/Computer Parts.xlsx
+++ b/Computer Parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sspring963\Documents\UiPath\BlankProcess\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sspring963\Documents\UiPath\ProductComparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,12 +17,12 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Results" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Computer parts</t>
   </si>
@@ -189,40 +189,52 @@
     <t>BestBuy Price</t>
   </si>
   <si>
-    <t>$1,099.99</t>
-  </si>
-  <si>
-    <t>$449.00</t>
-  </si>
-  <si>
-    <t>$299.00</t>
-  </si>
-  <si>
-    <t>$149.99</t>
-  </si>
-  <si>
-    <t>$159.99</t>
-  </si>
-  <si>
-    <t>$79.99</t>
-  </si>
-  <si>
-    <t>$84.99</t>
-  </si>
-  <si>
-    <t>$219.99</t>
-  </si>
-  <si>
-    <t>$157.99</t>
-  </si>
-  <si>
-    <t>$164.99</t>
-  </si>
-  <si>
-    <t>$199.99</t>
-  </si>
-  <si>
-    <t>$49.99</t>
+    <t>NewEgg Price</t>
+  </si>
+  <si>
+    <t>399.99</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>279.99</t>
+  </si>
+  <si>
+    <t>149.99</t>
+  </si>
+  <si>
+    <t>159.99</t>
+  </si>
+  <si>
+    <t>79.99</t>
+  </si>
+  <si>
+    <t>84.99</t>
+  </si>
+  <si>
+    <t>99.99</t>
+  </si>
+  <si>
+    <t>219.99</t>
+  </si>
+  <si>
+    <t>174.99</t>
+  </si>
+  <si>
+    <t>157.99</t>
+  </si>
+  <si>
+    <t>164.99</t>
+  </si>
+  <si>
+    <t>199.99</t>
+  </si>
+  <si>
+    <t>179.99</t>
+  </si>
+  <si>
+    <t>53.99</t>
   </si>
 </sst>
 </file>
@@ -286,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -299,6 +311,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,11 +530,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
@@ -726,126 +739,6 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -861,7 +754,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
@@ -1047,96 +940,106 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25 E25"/>
+      <selection activeCell="D2" sqref="D2 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.88671875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="51.77734375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="5">
         <v>192876928790</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3" s="5">
         <v>730143312714</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5">
       <c r="A4" s="5">
         <v>730143312042</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:5">
       <c r="A5" s="5">
         <v>735858446006</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:5">
       <c r="A6" s="6">
         <v>840006604839</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:5">
       <c r="A7" s="7">
         <v>824142218600</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:5">
       <c r="A8" s="6">
         <v>840006636656</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:5">
       <c r="A9" s="5">
         <v>843591058124</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:5">
       <c r="A10" s="5">
         <v>824142242148</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:5">
       <c r="A11" s="5">
         <v>840006630609</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:5">
       <c r="A12" s="5">
         <v>840006616696</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:5">
       <c r="A13" s="5">
         <v>840006627470</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:5">
       <c r="A14" s="5">
         <v>730143309936</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:5">
       <c r="A15" s="5">
         <v>889523019023</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:5">
       <c r="A16" s="5">
         <v>848354033103</v>
       </c>
@@ -1153,152 +1056,212 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>192876928790</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="1">
+        <v>1099.99</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>730143312714</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>449</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>730143312042</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>735858446006</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>840006604839</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>824142218600</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>840006636656</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>843591058124</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>824142242148</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>840006630609</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>840006616696</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>840006627470</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>730143309936</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>889523019023</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>848354033103</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>718037815367</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>66</v>
+      <c r="B17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included get prices from newegg
</commit_message>
<xml_diff>
--- a/Computer Parts.xlsx
+++ b/Computer Parts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="9564" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="9564" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VeryGood" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
   <si>
     <t>Computer parts</t>
   </si>
@@ -192,21 +192,42 @@
     <t>NewEgg Price</t>
   </si>
   <si>
+    <t>1099.99</t>
+  </si>
+  <si>
+    <t>1,129.99</t>
+  </si>
+  <si>
+    <t>449</t>
+  </si>
+  <si>
     <t>399.99</t>
   </si>
   <si>
+    <t>429.00</t>
+  </si>
+  <si>
     <t>299</t>
   </si>
   <si>
     <t>279.99</t>
   </si>
   <si>
+    <t>299.99</t>
+  </si>
+  <si>
     <t>149.99</t>
   </si>
   <si>
     <t>159.99</t>
   </si>
   <si>
+    <t>246.23</t>
+  </si>
+  <si>
+    <t>158.77</t>
+  </si>
+  <si>
     <t>79.99</t>
   </si>
   <si>
@@ -222,6 +243,9 @@
     <t>174.99</t>
   </si>
   <si>
+    <t>216.98</t>
+  </si>
+  <si>
     <t>157.99</t>
   </si>
   <si>
@@ -231,17 +255,83 @@
     <t>199.99</t>
   </si>
   <si>
+    <t>238.36</t>
+  </si>
+  <si>
     <t>179.99</t>
   </si>
   <si>
+    <t>49.99</t>
+  </si>
+  <si>
     <t>53.99</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>ASUS ROG Strix GeForce RTX 3080 DirectX 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD Ryzen 7 5800X 8-Core 3.8 GHz Socket AM4 105W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD Ryzen 5 5600X 6-Core 3.7 GHz Socket AM4 65W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel Core i5-10400 Comet Lake 6-Core 2.9 GHz LGA 1200 65W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORSAIR RMx Series (2021) RM850x CP-9020200-NA 850W </t>
+  </si>
+  <si>
+    <t>MSI MPG B550 GAMING PLUS AM4 AMD B550 SATA 6Gb/s ATX AMD Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORSAIR iCUE SP120 RGB ELITE Performance 120mm PWM Triple Fan </t>
+  </si>
+  <si>
+    <t>CORSAIR CX-M Series CX650M 650W 80 PLUS BRONZE</t>
+  </si>
+  <si>
+    <t>MSI Z590 PRO WIFI LGA 1200 Intel Z590 SATA 6Gb/s ATX Intel Motherboard</t>
+  </si>
+  <si>
+    <t>CORSAIR iCUE H100i ELITE CAPELLIX WHITE</t>
+  </si>
+  <si>
+    <t>CORSAIR iCUE H150i RGB PRO XT, 360mm Radiator, Triple 120mm PWM Fans</t>
+  </si>
+  <si>
+    <t>Corsair 5000D Airflow Tempered Glass Mid-Tower ATX PC Case</t>
+  </si>
+  <si>
+    <t>AMD RYZEN 5 3600 6-Core 3.6 GHz (4.2 GHz Max Boost) Socket AM4 65W</t>
+  </si>
+  <si>
+    <t>GIGABYTE X570 UD AMD Ryzen 3000 PCIe 4.0 SATA 6Gb/s USB 3.2 AMD X570 ATX Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.SKILL Ripjaws V Series 32GB (2 x 16GB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WD Desktop Mainstream WDBH2D0020HNC-NRSN 2TB </t>
+  </si>
+  <si>
+    <t>BestBuy URL</t>
+  </si>
+  <si>
+    <t>MicroCenter URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -258,6 +348,12 @@
       <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="&quot;Open Sans&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -298,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -308,10 +404,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +637,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
@@ -585,13 +688,6 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -606,10 +702,6 @@
       <c r="D3" s="1">
         <v>730143309936</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -627,9 +719,6 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -638,7 +727,6 @@
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5"/>
       <c r="D5" s="1">
         <v>848354033103</v>
       </c>
@@ -648,8 +736,6 @@
       <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -658,14 +744,9 @@
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6"/>
       <c r="D6" s="1">
         <v>718037815367</v>
       </c>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -677,15 +758,12 @@
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7"/>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7"/>
       <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H7"/>
       <c r="K7" s="2" t="s">
         <v>19</v>
       </c>
@@ -700,13 +778,9 @@
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
       <c r="G8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H8"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -718,27 +792,17 @@
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9"/>
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9"/>
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -754,7 +818,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
@@ -928,7 +992,6 @@
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -940,114 +1003,193 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2 D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="51.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="71.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5">
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="8">
         <v>192876928790</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="8">
         <v>730143312714</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="8">
         <v>730143312042</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="8">
         <v>735858446006</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="9">
         <v>840006604839</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="7">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="5">
         <v>824142218600</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6">
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="9">
         <v>840006636656</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="8">
         <v>843591058124</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="8">
         <v>824142242148</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="5">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="8">
         <v>840006630609</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="8">
         <v>840006616696</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="5">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="8">
         <v>840006627470</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="5">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="8">
         <v>730143309936</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="5">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="8">
         <v>889523019023</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="5">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="8">
         <v>848354033103</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="5">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="8">
         <v>718037815367</v>
       </c>
+      <c r="D17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1058,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1092,175 +1234,223 @@
       <c r="A2" s="1">
         <v>192876928790</v>
       </c>
-      <c r="B2" s="1">
-        <v>1099.99</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>730143312714</v>
       </c>
-      <c r="B3" s="1">
-        <v>449</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>56</v>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>730143312042</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>58</v>
+      <c r="B4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>735858446006</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>60</v>
+      <c r="B5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>840006604839</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>824142218600</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>60</v>
+      <c r="B7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>840006636656</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>843591058124</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>63</v>
+      <c r="B9" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="10">
+        <v>99.99</v>
+      </c>
+      <c r="D9" s="1">
+        <v>94.99</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>824142242148</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>64</v>
+      <c r="B10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1">
+        <v>219.99</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>840006630609</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>65</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>840006616696</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>65</v>
+      <c r="B12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>840006627470</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>60</v>
+      <c r="B13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>730143309936</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>64</v>
+      <c r="B14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>889523019023</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>69</v>
+      <c r="C15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>848354033103</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>718037815367</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scraping url for bestbuy, microcenter
</commit_message>
<xml_diff>
--- a/Computer Parts.xlsx
+++ b/Computer Parts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="9564" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="9564" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="VeryGood" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="111">
   <si>
     <t>Computer parts</t>
   </si>
@@ -183,63 +183,141 @@
     <t>Cougar MX330-X</t>
   </si>
   <si>
+    <t>Product Name</t>
+  </si>
+  <si>
     <t>WORKING UPCS</t>
   </si>
   <si>
     <t>BestBuy Price</t>
   </si>
   <si>
+    <t>BestBuy URL</t>
+  </si>
+  <si>
+    <t>MicroCenter URL</t>
+  </si>
+  <si>
     <t>NewEgg Price</t>
   </si>
   <si>
+    <t>ASUS ROG Strix GeForce RTX 3080 DirectX 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD Ryzen 7 5800X 8-Core 3.8 GHz Socket AM4 105W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMD Ryzen 5 5600X 6-Core 3.7 GHz Socket AM4 65W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel Core i5-10400 Comet Lake 6-Core 2.9 GHz LGA 1200 65W </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORSAIR RMx Series (2021) RM850x CP-9020200-NA 850W </t>
+  </si>
+  <si>
+    <t>MSI MPG B550 GAMING PLUS AM4 AMD B550 SATA 6Gb/s ATX AMD Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORSAIR iCUE SP120 RGB ELITE Performance 120mm PWM Triple Fan </t>
+  </si>
+  <si>
+    <t>CORSAIR CX-M Series CX650M 650W 80 PLUS BRONZE</t>
+  </si>
+  <si>
+    <t>MSI Z590 PRO WIFI LGA 1200 Intel Z590 SATA 6Gb/s ATX Intel Motherboard</t>
+  </si>
+  <si>
+    <t>CORSAIR iCUE H100i ELITE CAPELLIX WHITE</t>
+  </si>
+  <si>
+    <t>CORSAIR iCUE H150i RGB PRO XT, 360mm Radiator, Triple 120mm PWM Fans</t>
+  </si>
+  <si>
+    <t>Corsair 5000D Airflow Tempered Glass Mid-Tower ATX PC Case</t>
+  </si>
+  <si>
+    <t>AMD RYZEN 5 3600 6-Core 3.6 GHz (4.2 GHz Max Boost) Socket AM4 65W</t>
+  </si>
+  <si>
+    <t>GIGABYTE X570 UD AMD Ryzen 3000 PCIe 4.0 SATA 6Gb/s USB 3.2 AMD X570 ATX Motherboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G.SKILL Ripjaws V Series 32GB (2 x 16GB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WD Desktop Mainstream WDBH2D0020HNC-NRSN 2TB </t>
+  </si>
+  <si>
     <t>1099.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/asus-geforce-rtx-3080-10gb-gddr6x-pci-express-4-0-strix-graphics-card-black/6432445.p?skuId=6432445</t>
+  </si>
+  <si>
     <t>1,129.99</t>
   </si>
   <si>
-    <t>449</t>
+    <t>https://www.bestbuy.com//site/amd-ryzen-7-5800x-4th-gen-8-core-16-threads-unlocked-desktop-processor-without-cooler/6439000.p?skuId=6439000</t>
   </si>
   <si>
     <t>399.99</t>
   </si>
   <si>
-    <t>429.00</t>
-  </si>
-  <si>
     <t>299</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/amd-ryzen-5-5600x-4th-gen-6-core-12-threads-unlocked-desktop-processor-with-wraith-stealth-cooler/6438943.p?skuId=6438943</t>
+  </si>
+  <si>
     <t>279.99</t>
   </si>
   <si>
-    <t>299.99</t>
-  </si>
-  <si>
     <t>149.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/intel-core-i5-10400-10th-generation-6-core-12-thread-2-9-ghz-4-3-ghz-turbo-socket-lga1200-locked-desktop-processor/6411498.p?skuId=6411498</t>
+  </si>
+  <si>
     <t>159.99</t>
   </si>
   <si>
-    <t>246.23</t>
+    <t>https://www.bestbuy.com//site/corsair-rmx-series-rm850x-80-plus-gold-fully-modular-atx-power-supply-black/6459244.p?skuId=6459244</t>
   </si>
   <si>
     <t>158.77</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/msi-b550-gaming-plus-socket-am4-usb-c-gen-2-amd-atx-gaming-motherboard-pcie-gen-4-black/6424047.p?skuId=6424047</t>
+  </si>
+  <si>
     <t>79.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/corsair-icue-sp120-rgb-elite-performance-120mm-pwm-triple-fan-kit-with-icue-lighting-node-core-black/6454636.p?skuId=6454636</t>
+  </si>
+  <si>
     <t>84.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/corsair-cx-m-series-650w-atx12v-2-4-eps12v-2-92-80-plus-bronze-modular-power-supply-matte-black/5845214.p?skuId=5845214</t>
+  </si>
+  <si>
     <t>99.99</t>
   </si>
   <si>
+    <t>94.99</t>
+  </si>
+  <si>
     <t>219.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/msi-z590-pro-wifi-socket-lga1200-intel-motherboard/6455367.p?skuId=6455367</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com//site/corsair-icue-h100i-elite-capellix-240mm-radiator-liquid-cpu-cooler-white/6449964.p?skuId=6449964</t>
+  </si>
+  <si>
     <t>174.99</t>
   </si>
   <si>
@@ -249,12 +327,21 @@
     <t>157.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/corsair-icue-h150i-360mm-radiator-cpu-liquid-cooling-system-black/6414216.p?skuId=6414216</t>
+  </si>
+  <si>
     <t>164.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/corsair-5000d-airflow-atx-mid-tower-black/6453227.p?skuId=6453227</t>
+  </si>
+  <si>
     <t>199.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/amd-ryzen-5-3600-3rd-generation-6-core-12-thread-3-6-ghz-4-2-ghz-max-boost-socket-am4-unlocked-desktop-processor/6356278.p?skuId=6356278</t>
+  </si>
+  <si>
     <t>238.36</t>
   </si>
   <si>
@@ -264,64 +351,10 @@
     <t>49.99</t>
   </si>
   <si>
+    <t>https://www.bestbuy.com//site/wd-blue-2tb-internal-sata-hard-drive-for-desktops/9312076.p?skuId=9312076</t>
+  </si>
+  <si>
     <t>53.99</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>ASUS ROG Strix GeForce RTX 3080 DirectX 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMD Ryzen 7 5800X 8-Core 3.8 GHz Socket AM4 105W </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMD Ryzen 5 5600X 6-Core 3.7 GHz Socket AM4 65W </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intel Core i5-10400 Comet Lake 6-Core 2.9 GHz LGA 1200 65W </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORSAIR RMx Series (2021) RM850x CP-9020200-NA 850W </t>
-  </si>
-  <si>
-    <t>MSI MPG B550 GAMING PLUS AM4 AMD B550 SATA 6Gb/s ATX AMD Motherboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORSAIR iCUE SP120 RGB ELITE Performance 120mm PWM Triple Fan </t>
-  </si>
-  <si>
-    <t>CORSAIR CX-M Series CX650M 650W 80 PLUS BRONZE</t>
-  </si>
-  <si>
-    <t>MSI Z590 PRO WIFI LGA 1200 Intel Z590 SATA 6Gb/s ATX Intel Motherboard</t>
-  </si>
-  <si>
-    <t>CORSAIR iCUE H100i ELITE CAPELLIX WHITE</t>
-  </si>
-  <si>
-    <t>CORSAIR iCUE H150i RGB PRO XT, 360mm Radiator, Triple 120mm PWM Fans</t>
-  </si>
-  <si>
-    <t>Corsair 5000D Airflow Tempered Glass Mid-Tower ATX PC Case</t>
-  </si>
-  <si>
-    <t>AMD RYZEN 5 3600 6-Core 3.6 GHz (4.2 GHz Max Boost) Socket AM4 65W</t>
-  </si>
-  <si>
-    <t>GIGABYTE X570 UD AMD Ryzen 3000 PCIe 4.0 SATA 6Gb/s USB 3.2 AMD X570 ATX Motherboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G.SKILL Ripjaws V Series 32GB (2 x 16GB) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WD Desktop Mainstream WDBH2D0020HNC-NRSN 2TB </t>
-  </si>
-  <si>
-    <t>BestBuy URL</t>
-  </si>
-  <si>
-    <t>MicroCenter URL</t>
   </si>
 </sst>
 </file>
@@ -394,8 +427,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -404,17 +438,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,172 +667,211 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="15.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="2" customWidth="1"/>
+    <col min="3" max="6" width="15.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>730143309936</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>889523019023</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5"/>
+      <c r="D5" s="2">
         <v>848354033103</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="G5"/>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1">
+      <c r="C6"/>
+      <c r="D6" s="2">
         <v>718037815367</v>
       </c>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7"/>
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="F7"/>
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="H7"/>
+      <c r="K7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9"/>
+      <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="F9"/>
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="H9"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -818,180 +887,181 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>730143311731</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>410574000038</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>889349672068</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>649528790064</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>718037856254</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>740617261219</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>843368064570</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>695975089985</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1005,191 +1075,191 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4 H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="20.109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="71.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="12" t="s">
+      <c r="F1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6">
         <v>192876928790</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6">
         <v>730143312714</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="8">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="6">
         <v>730143312042</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="6">
         <v>735858446006</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="13" t="s">
-        <v>86</v>
+      <c r="A6" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B6" s="9">
         <v>840006604839</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="A7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="10">
         <v>824142218600</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="13" t="s">
-        <v>88</v>
+      <c r="A8" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B8" s="9">
         <v>840006636656</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="8">
+      <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="6">
         <v>843591058124</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="8">
+      <c r="A10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="6">
         <v>824142242148</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="8">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="6">
         <v>840006630609</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="8">
+      <c r="A12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="6">
         <v>840006616696</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="8">
+      <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="6">
         <v>840006627470</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="6">
         <v>730143309936</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="8">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="6">
         <v>889523019023</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="8">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="6">
         <v>848354033103</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="8">
+      <c r="A17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="6">
         <v>718037815367</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1198,260 +1268,381 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2">
         <v>192876928790</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
+      <c r="G2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2">
         <v>730143312714</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
+      <c r="C3" s="11">
+        <v>449</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="11">
         <v>730143312042</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="11">
+        <v>735858446006</v>
+      </c>
+      <c r="C5" s="11">
+        <v>149.99</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="2">
+        <v>159.99</v>
+      </c>
+      <c r="G5" s="2">
+        <v>246.23</v>
+      </c>
+      <c r="K5" s="12">
+        <f>MIN(C5:G5)</f>
+        <v>149.99</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>735858446006</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="11">
+        <v>840006604839</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="B7" s="11">
+        <v>824142218600</v>
+      </c>
+      <c r="C7" s="11">
+        <v>159.99</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="2">
+        <v>159.99</v>
+      </c>
+      <c r="G7" s="2">
+        <v>159.99</v>
+      </c>
+      <c r="K7" s="12">
+        <f>MIN(C7:G7)</f>
+        <v>159.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B8" s="11">
+        <v>840006636656</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>840006604839</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B9" s="11">
+        <v>843591058124</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="11">
+        <v>824142242148</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="11">
+        <v>840006630609</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="11">
+        <v>840006616696</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="11">
+        <v>840006627470</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="11">
+        <v>730143309936</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="11">
+        <v>889523019023</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>824142218600</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1">
-        <v>840006636656</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="D15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1">
-        <v>843591058124</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="10">
-        <v>99.99</v>
-      </c>
-      <c r="D9" s="1">
-        <v>94.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1">
-        <v>824142242148</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="1">
-        <v>219.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>840006630609</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="G15" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
-        <v>840006616696</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="B16" s="11">
+        <v>848354033103</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1">
-        <v>840006627470</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1">
-        <v>730143309936</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1">
-        <v>889523019023</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1">
-        <v>848354033103</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="B17" s="11">
         <v>718037815367</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>70</v>
+      <c r="C17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented found min and send email
</commit_message>
<xml_diff>
--- a/Computer Parts.xlsx
+++ b/Computer Parts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sspring963\Documents\UiPath\ProductComparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanl\P2\P2_Team_SSJN\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BF9BCF-4675-443A-9B02-A9960667B5F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="23232" windowHeight="9564" firstSheet="0" activeTab="3"/>
+    <x:workbookView xWindow="4065" yWindow="4365" windowWidth="21600" windowHeight="11835" firstSheet="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="VeryGood" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,23 @@
     <x:sheet name="Results" sheetId="7" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="152511"/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </x:ext>
+  </x:extLst>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <x:si>
     <x:t>Computer parts</x:t>
   </x:si>
@@ -250,37 +262,88 @@
     <x:t xml:space="preserve">WD Desktop Mainstream WDBH2D0020HNC-NRSN 2TB </x:t>
   </x:si>
   <x:si>
+    <x:t>1099.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/asus-geforce-rtx-3080-10gb-gddr6x-pci-express-4-0-strix-graphics-card-black/6432445.p?skuId=6432445</x:t>
+  </x:si>
+  <x:si>
     <x:t>1,129.99</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.newegg.com/asus-geforce-rtx-3080-rog-strix-rtx3080-o10g-gaming/p/N82E16814126457?Description=192876928790&amp;cm_re=192876928790-_-14-126-457-_-Product&amp;quicklink=true</x:t>
+    <x:t>https://www.newegg.com/asus-geforce-rtx-3080-rog-strix-rtx3080-o10g-gaming/p/N82E16814126457?Description=192876928790&amp;cm_re=192876928790-_-14-126-457-_-Product</x:t>
+  </x:si>
+  <x:si>
+    <x:t>449</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/amd-ryzen-7-5800x-4th-gen-8-core-16-threads-unlocked-desktop-processor-without-cooler/6439000.p?skuId=6439000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>399.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/630284/amd-ryzen-7-5800x-vermeer-38ghz-8-core-am4-boxed-processor</x:t>
   </x:si>
   <x:si>
     <x:t>429.00</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.newegg.com/amd-ryzen-7-5800x/p/N82E16819113665?Description=730143312714&amp;cm_re=730143312714-_-19-113-665-_-Product&amp;quicklink=true</x:t>
+    <x:t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118183</x:t>
+  </x:si>
+  <x:si>
+    <x:t>299</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/amd-ryzen-5-5600x-4th-gen-6-core-12-threads-unlocked-desktop-processor-with-wraith-stealth-cooler/6438943.p?skuId=6438943</x:t>
+  </x:si>
+  <x:si>
+    <x:t>279.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/630285/amd-ryzen-5-5600x-vermeer-37ghz-6-core-am4-boxed-processor-with-wraith-stealth-cooler</x:t>
   </x:si>
   <x:si>
     <x:t>299.99</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.newegg.com/amd-ryzen-5-5600x/p/N82E16819113666?Description=730143312042&amp;cm_re=730143312042-_-19-113-666-_-Product&amp;quicklink=true</x:t>
-  </x:si>
-  <x:si>
-    <x:t>246.23</x:t>
+    <x:t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>164.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/intel-core-i5-10400-10th-generation-6-core-12-thread-2-9-ghz-4-3-ghz-turbo-socket-lga1200-locked-desktop-processor/6411498.p?skuId=6411498</x:t>
+  </x:si>
+  <x:si>
+    <x:t>159.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/622904/intel-core-i5-10400-comet-lake-29ghz-six-core-lga-1200-boxed-processor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>169.99</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.newegg.com/intel-core-i5-10400-core-i5-10th-gen/p/N82E16819118135?Description=735858446006&amp;cm_re=735858446006-_-19-118-135-_-Product&amp;quicklink=true</x:t>
   </x:si>
   <x:si>
-    <x:t>158.77</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.newegg.com/corsair-cx550f-rgb-cp-9020216-na-550w/p/N82E16817139265</x:t>
-  </x:si>
-  <x:si>
-    <x:t>159.99</x:t>
+    <x:t>149.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/corsair-rmx-series-rm850x-80-plus-gold-fully-modular-atx-power-supply-black/6459244.p?skuId=6459244</x:t>
+  </x:si>
+  <x:si>
+    <x:t>159.17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/corsair-rmx-series-rm850x-cp-9020200-na-850w/p/N82E16817139272?Description=840006604839&amp;cm_re=840006604839-_-17-139-272-_-Product</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/msi-b550-gaming-plus-socket-am4-usb-c-gen-2-amd-atx-gaming-motherboard-pcie-gen-4-black/6424047.p?skuId=6424047</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/625046/msi-b550-mpg-gaming-plus-amd-am4-atx-motherboard</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.newegg.com/msi-mpg-b550-gaming-plus/p/N82E16813144325?Description=824142218600&amp;cm_re=824142218600-_-13-144-325-_-Product</x:t>
@@ -289,65 +352,134 @@
     <x:t>79.99</x:t>
   </x:si>
   <x:si>
+    <x:t>https://www.bestbuy.com/site/corsair-icue-sp120-rgb-elite-performance-120mm-pwm-triple-fan-kit-with-icue-lighting-node-core-black/6454636.p?skuId=6454636</x:t>
+  </x:si>
+  <x:si>
+    <x:t>109.99</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.newegg.com/corsair-co-9050109-ww-case-fan/p/N82E16835181236?Description=840006636656&amp;cm_re=840006636656-_-35-181-236-_-Product</x:t>
   </x:si>
   <x:si>
     <x:t>94.99</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.newegg.com/corsair-cx-series-cx650m-650w/p/N82E16817139148?Description=843591058124&amp;cm_re=843591058124-_-17-139-148-_-Product</x:t>
+    <x:t>https://www.bestbuy.com/site/corsair-cx-m-series-650w-atx12v-2-4-eps12v-2-92-80-plus-bronze-modular-power-supply-matte-black/5845214.p?skuId=5845214</x:t>
+  </x:si>
+  <x:si>
+    <x:t>99.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/460288/corsair-cx650m-650-watt-80-plus-bronze-atx-semi-modular-power-supply</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/corsair-cx650f-rgb-cp-9020217-na-650w/p/N82E16817139263</x:t>
   </x:si>
   <x:si>
     <x:t>219.99</x:t>
   </x:si>
   <x:si>
+    <x:t>https://www.bestbuy.com/site/msi-z590-pro-wifi-socket-lga1200-intel-motherboard/6455367.p?skuId=6455367</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/634676/msi-z590-mag-pro-wifi-intel-lga-1200-atx-motherboard</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.newegg.com/p/N82E16813144391?Description=824142242148&amp;cm_re=824142242148-_-13-144-391-_-Product</x:t>
   </x:si>
   <x:si>
-    <x:t>216.98</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.newegg.com/rosewill-liquid-cooling-system/p/N82E16835200128</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.newegg.com/corsair-icue-h150i-rgb-pro-xt-liquid-cooling-system/p/N82E16835181192?Description=840006616696&amp;cm_re=840006616696-_-35-181-192-_-Product</x:t>
-  </x:si>
-  <x:si>
-    <x:t>164.99</x:t>
+    <x:t>https://www.bestbuy.com/site/corsair-icue-h100i-elite-capellix-240mm-radiator-liquid-cpu-cooler-white/6449964.p?skuId=6449964</x:t>
+  </x:si>
+  <x:si>
+    <x:t>174.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/632325/corsair-icue-h100i-elite-capellix-240mm-rgb-water-cooling-kit-white</x:t>
+  </x:si>
+  <x:si>
+    <x:t>175.22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/corsair-liquid-cooling-system-icue-h150i-elite-capellix/p/N82E16835181203</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/corsair-icue-h150i-360mm-radiator-cpu-liquid-cooling-system-black/6414216.p?skuId=6414216</x:t>
+  </x:si>
+  <x:si>
+    <x:t>179.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/617538/corsair-h150i-pro-xt-360mm-rgb-water-cooling-kit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>152.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/corsair-icue-h150i-rgb-pro-xt-liquid-cooling-system/p/N82E16835181192?Description=840006616696&amp;cm_re=840006616696-_-35-181-192-_-Product&amp;quicklink=true</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/corsair-5000d-airflow-atx-mid-tower-black/6453227.p?skuId=6453227</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/632020/corsair-5000d-airflow-tempered-glass-mid-tower-atx-computer-case-black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>226.99</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.newegg.com/black-corsair-5000d-airflow-atx-mid-tower/p/N82E16811139161?Description=840006627470&amp;cm_re=840006627470-_-11-139-161-_-Product</x:t>
   </x:si>
   <x:si>
-    <x:t>238.36</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.newegg.com/intel-core-i7-10700k-core-i7-10th-gen/p/N82E16819118183</x:t>
-  </x:si>
-  <x:si>
-    <x:t>179.99</x:t>
+    <x:t>199.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/amd-ryzen-5-3600-3rd-generation-6-core-12-thread-3-6-ghz-4-2-ghz-max-boost-socket-am4-unlocked-desktop-processor/6356278.p?skuId=6356278</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/608320/amd-ryzen-5-3600-matisse-36ghz-6-core-am4-boxed-processor-with-wraith-stealth-cooler</x:t>
+  </x:si>
+  <x:si>
+    <x:t>237.95</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/611186/gigabyte-x570-ud-amd-am4-atx-motherboard?ob=1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>172.10</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.newegg.com/gigabyte-x570-ud/p/N82E16813145168?Description=889523019023&amp;cm_re=889523019023-_-13-145-168-_-Product</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.newegg.com/g-skill-32gb-288-pin-ddr4-sdram/p/N82E16820232920</x:t>
-  </x:si>
-  <x:si>
-    <x:t>99.99</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.newegg.com/desktop-mainstream-wdbh2d0020hnc-nrsn-2tb/p/N82E16822236531?Description=718037815367&amp;cm_re=718037815367-_-22-236-531-_-Product</x:t>
+    <x:t>https://www.microcenter.com/product/636569/gskill-ripjaws-v-32gb-(2-x-16gb)-ddr4-3600-pc4-28800-cl18-dual-channel-desktop-memory-kit-f4-3600c18d-32gvk-black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/g-skill-32gb-288-pin-ddr4-sdram/p/N82E16820232091</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.bestbuy.com/site/wd-blue-2tb-internal-sata-hard-drive-for-desktops/9312076.p?skuId=9312076</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53.99</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.microcenter.com/product/415197/wd-blue-mainstream-2tb-5400rpm-sata-iii-6gb-s-35-internal-hard-drive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.newegg.com/desktop-mainstream-wdbh2d0020hnc-nrsn-2tb/p/N82E16822236531?Description=718037815367&amp;cm_re=718037815367-_-22-236-531-_-Product&amp;quicklink=true</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </x:numFmts>
-  <x:fonts count="5">
+  <x:fonts count="4">
     <x:font>
       <x:sz val="10"/>
       <x:color rgb="FF000000"/>
@@ -364,12 +496,6 @@
       <x:sz val="11"/>
       <x:color rgb="FF212529"/>
       <x:name val="&quot;Open Sans&quot;"/>
-    </x:font>
-    <x:font>
-      <x:sz val="10"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Arial"/>
-      <x:family val="2"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -414,7 +540,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="13">
+  <x:cellStyleXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -446,16 +572,9 @@
     <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="23">
+  <x:cellXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -470,7 +589,6 @@
     <x:xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -724,219 +842,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="0" summaryRight="0"/>
   </x:sheetPr>
   <x:dimension ref="A1:L10"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A13" sqref="A13 A13:A13"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="21.530625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="22.995781" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.109375" style="13" customWidth="1"/>
-    <x:col min="2" max="2" width="58.886719" style="13" customWidth="1"/>
-    <x:col min="3" max="6" width="15.109375" style="13" customWidth="1"/>
-    <x:col min="7" max="7" width="16.554688" style="13" customWidth="1"/>
-    <x:col min="8" max="8" width="15.886719" style="13" customWidth="1"/>
+    <x:col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
+    <x:col min="2" max="2" width="58.855469" style="11" customWidth="1"/>
+    <x:col min="3" max="6" width="15.140625" style="11" customWidth="1"/>
+    <x:col min="7" max="7" width="16.570312" style="11" customWidth="1"/>
+    <x:col min="8" max="8" width="15.855469" style="11" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="11" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="11" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="11" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="11" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="13" t="s">
+      <x:c r="E1" s="11" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="11" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="13" t="s">
+      <x:c r="G1" s="11" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="11" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="13" t="s">
+      <x:c r="I1" s="11" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="13" t="s">
+      <x:c r="J1" s="11" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="13" t="s">
+      <x:c r="K1" s="11" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="13" t="s">
+      <x:c r="L1" s="11" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A2" s="13" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B2" s="13" t="s"/>
-      <x:c r="C2" s="13" t="s"/>
-      <x:c r="D2" s="13" t="s"/>
-      <x:c r="E2" s="13" t="s"/>
-      <x:c r="F2" s="13" t="s"/>
-      <x:c r="G2" s="13" t="s"/>
-      <x:c r="H2" s="13" t="s"/>
+      <x:c r="B2" s="11" t="s"/>
+      <x:c r="C2" s="11" t="s"/>
+      <x:c r="D2" s="11" t="s"/>
+      <x:c r="E2" s="11" t="s"/>
+      <x:c r="F2" s="11" t="s"/>
+      <x:c r="G2" s="11" t="s"/>
+      <x:c r="H2" s="11" t="s"/>
     </x:row>
     <x:row r="3" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A3" s="13" t="s">
+      <x:c r="A3" s="11" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B3" s="13" t="s">
+      <x:c r="B3" s="11" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C3" s="13" t="s">
+      <x:c r="C3" s="11" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="D3" s="13" t="n">
+      <x:c r="D3" s="11" t="n">
         <x:v>730143309936</x:v>
       </x:c>
-      <x:c r="E3" s="13" t="s"/>
-      <x:c r="F3" s="13" t="s"/>
-      <x:c r="G3" s="13" t="s"/>
-      <x:c r="H3" s="13" t="s"/>
+      <x:c r="E3" s="11" t="s"/>
+      <x:c r="F3" s="11" t="s"/>
+      <x:c r="G3" s="11" t="s"/>
+      <x:c r="H3" s="11" t="s"/>
     </x:row>
     <x:row r="4" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A4" s="13" t="s">
+      <x:c r="A4" s="11" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B4" s="13" t="s">
+      <x:c r="B4" s="11" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C4" s="13" t="s">
+      <x:c r="C4" s="11" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D4" s="13" t="n">
+      <x:c r="D4" s="11" t="n">
         <x:v>889523019023</x:v>
       </x:c>
-      <x:c r="E4" s="13" t="s">
+      <x:c r="E4" s="11" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F4" s="13" t="s"/>
-      <x:c r="G4" s="13" t="s"/>
-      <x:c r="H4" s="13" t="s"/>
+      <x:c r="F4" s="11" t="s"/>
+      <x:c r="G4" s="11" t="s"/>
+      <x:c r="H4" s="11" t="s"/>
     </x:row>
     <x:row r="5" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A5" s="13" t="s">
+      <x:c r="A5" s="11" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B5" s="13" t="s">
+      <x:c r="B5" s="11" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C5" s="13" t="s"/>
-      <x:c r="D5" s="13" t="n">
+      <x:c r="C5" s="11" t="s"/>
+      <x:c r="D5" s="11" t="n">
         <x:v>848354033103</x:v>
       </x:c>
-      <x:c r="E5" s="13" t="s">
+      <x:c r="E5" s="11" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F5" s="13" t="s">
+      <x:c r="F5" s="11" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="G5" s="13" t="s"/>
-      <x:c r="H5" s="13" t="s"/>
+      <x:c r="G5" s="11" t="s"/>
+      <x:c r="H5" s="11" t="s"/>
     </x:row>
     <x:row r="6" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A6" s="13" t="s">
+      <x:c r="A6" s="11" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B6" s="13" t="s">
+      <x:c r="B6" s="11" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C6" s="13" t="s"/>
-      <x:c r="D6" s="13" t="n">
+      <x:c r="C6" s="11" t="s"/>
+      <x:c r="D6" s="11" t="n">
         <x:v>718037815367</x:v>
       </x:c>
-      <x:c r="E6" s="13" t="s"/>
-      <x:c r="F6" s="13" t="s"/>
-      <x:c r="G6" s="13" t="s"/>
-      <x:c r="H6" s="13" t="s"/>
+      <x:c r="E6" s="11" t="s"/>
+      <x:c r="F6" s="11" t="s"/>
+      <x:c r="G6" s="11" t="s"/>
+      <x:c r="H6" s="11" t="s"/>
     </x:row>
     <x:row r="7" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A7" s="13" t="s">
+      <x:c r="A7" s="11" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B7" s="13" t="s">
+      <x:c r="B7" s="11" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C7" s="13" t="s">
+      <x:c r="C7" s="11" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="D7" s="13" t="s"/>
-      <x:c r="E7" s="13" t="s">
+      <x:c r="D7" s="11" t="s"/>
+      <x:c r="E7" s="11" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F7" s="13" t="s"/>
-      <x:c r="G7" s="14" t="s">
+      <x:c r="F7" s="11" t="s"/>
+      <x:c r="G7" s="12" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="H7" s="13" t="s"/>
-      <x:c r="K7" s="14" t="s">
+      <x:c r="H7" s="11" t="s"/>
+      <x:c r="K7" s="12" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A8" s="13" t="s">
+      <x:c r="A8" s="11" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B8" s="13" t="s">
+      <x:c r="B8" s="11" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C8" s="13" t="s">
+      <x:c r="C8" s="11" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D8" s="13" t="s"/>
-      <x:c r="E8" s="13" t="s"/>
-      <x:c r="F8" s="13" t="s"/>
-      <x:c r="G8" s="14" t="s">
+      <x:c r="D8" s="11" t="s"/>
+      <x:c r="E8" s="11" t="s"/>
+      <x:c r="F8" s="11" t="s"/>
+      <x:c r="G8" s="12" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="H8" s="13" t="s"/>
+      <x:c r="H8" s="11" t="s"/>
     </x:row>
     <x:row r="9" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A9" s="13" t="s">
+      <x:c r="A9" s="11" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B9" s="13" t="s">
+      <x:c r="B9" s="11" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C9" s="13" t="s">
+      <x:c r="C9" s="11" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="D9" s="13" t="s"/>
-      <x:c r="E9" s="13" t="s">
+      <x:c r="D9" s="11" t="s"/>
+      <x:c r="E9" s="11" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F9" s="13" t="s"/>
-      <x:c r="G9" s="14" t="s">
+      <x:c r="F9" s="11" t="s"/>
+      <x:c r="G9" s="12" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="H9" s="13" t="s"/>
+      <x:c r="H9" s="11" t="s"/>
     </x:row>
     <x:row r="10" spans="1:12" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A10" s="13" t="s">
+      <x:c r="A10" s="11" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B10" s="13" t="s"/>
-      <x:c r="C10" s="13" t="s"/>
-      <x:c r="D10" s="13" t="s"/>
-      <x:c r="E10" s="13" t="s"/>
-      <x:c r="F10" s="13" t="s"/>
-      <x:c r="G10" s="13" t="s"/>
-      <x:c r="H10" s="13" t="s"/>
+      <x:c r="B10" s="11" t="s"/>
+      <x:c r="C10" s="11" t="s"/>
+      <x:c r="D10" s="11" t="s"/>
+      <x:c r="E10" s="11" t="s"/>
+      <x:c r="F10" s="11" t="s"/>
+      <x:c r="G10" s="11" t="s"/>
+      <x:c r="H10" s="11" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:12">
+      <x:c r="A13" s="11" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -948,189 +1071,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="0" summaryRight="0"/>
   </x:sheetPr>
   <x:dimension ref="A1:N11"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A14" sqref="A14 A14:A14"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="21.530625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="22.995781" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.109375" style="13" customWidth="1"/>
-    <x:col min="2" max="2" width="58.886719" style="13" customWidth="1"/>
+    <x:col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
+    <x:col min="2" max="2" width="58.855469" style="11" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="11" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="11" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="11" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="11" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="13" t="s">
+      <x:c r="E1" s="11" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="11" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="G1" s="13" t="s">
+      <x:c r="G1" s="11" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="11" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="I1" s="14" t="s">
+      <x:c r="I1" s="12" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="J1" s="14" t="s">
+      <x:c r="J1" s="12" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="K1" s="14" t="s">
+      <x:c r="K1" s="12" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="L1" s="14" t="s">
+      <x:c r="L1" s="12" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="M1" s="14" t="s">
+      <x:c r="M1" s="12" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="N1" s="14" t="s">
+      <x:c r="N1" s="12" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A2" s="13" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B2" s="15" t="s">
+      <x:c r="B2" s="13" t="s">
         <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A3" s="13" t="s">
+      <x:c r="A3" s="11" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B3" s="13" t="s">
+      <x:c r="B3" s="11" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="C3" s="13" t="s">
+      <x:c r="C3" s="11" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="D3" s="13" t="n">
+      <x:c r="D3" s="11" t="n">
         <x:v>730143311731</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A4" s="13" t="s">
+      <x:c r="A4" s="11" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="B4" s="13" t="s">
+      <x:c r="B4" s="11" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C4" s="13" t="s">
+      <x:c r="C4" s="11" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="D4" s="13" t="n">
+      <x:c r="D4" s="11" t="n">
         <x:v>410574000038</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A5" s="13" t="s">
+      <x:c r="A5" s="11" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B5" s="13" t="s">
+      <x:c r="B5" s="11" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C5" s="13" t="s">
+      <x:c r="C5" s="11" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="D5" s="13" t="n">
+      <x:c r="D5" s="11" t="n">
         <x:v>889349672068</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A6" s="13" t="s">
+      <x:c r="A6" s="11" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B6" s="13" t="s">
+      <x:c r="B6" s="11" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="C6" s="13" t="s">
+      <x:c r="C6" s="11" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="D6" s="13" t="n">
+      <x:c r="D6" s="11" t="n">
         <x:v>649528790064</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A7" s="13" t="s">
+      <x:c r="A7" s="11" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B7" s="13" t="s">
+      <x:c r="B7" s="11" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="C7" s="14" t="s">
+      <x:c r="C7" s="12" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="D7" s="13" t="n">
+      <x:c r="D7" s="11" t="n">
         <x:v>718037856254</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A8" s="13" t="s">
+      <x:c r="A8" s="11" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B8" s="13" t="s">
+      <x:c r="B8" s="11" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="C8" s="13" t="s">
+      <x:c r="C8" s="11" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="D8" s="13" t="n">
+      <x:c r="D8" s="11" t="n">
         <x:v>740617261219</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A9" s="13" t="s">
+      <x:c r="A9" s="11" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B9" s="13" t="s">
+      <x:c r="B9" s="11" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C9" s="13" t="s">
+      <x:c r="C9" s="11" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="D9" s="16" t="n">
+      <x:c r="D9" s="14" t="n">
         <x:v>843368064570</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A10" s="13" t="s">
+      <x:c r="A10" s="11" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="B10" s="13" t="s">
+      <x:c r="B10" s="11" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="C10" s="13" t="s">
+      <x:c r="C10" s="11" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="D10" s="13" t="n">
+      <x:c r="D10" s="11" t="n">
         <x:v>695975089985</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:14" customFormat="1" ht="15.75" customHeight="1">
-      <x:c r="A11" s="13" t="s">
+      <x:c r="A11" s="11" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="B11" s="13" t="s"/>
+      <x:c r="B11" s="11" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:14">
+      <x:c r="A14" s="11" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -1142,7 +1270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="0" summaryRight="0"/>
   </x:sheetPr>
@@ -1152,187 +1280,187 @@
       <x:selection activeCell="H4" sqref="H4 H4:H4"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultColWidth="21.530625" defaultRowHeight="15.75" customHeight="1"/>
+  <x:sheetFormatPr defaultColWidth="22.995781" defaultRowHeight="15.75" customHeight="1"/>
   <x:cols>
-    <x:col min="1" max="1" width="71.554688" style="13" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="3" width="16.554688" style="13" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="71.570312" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="3" width="16.570312" style="11" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="11" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="B1" s="18" t="s">
+      <x:c r="B1" s="16" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="C1" s="19" t="s">
+      <x:c r="C1" s="17" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="11" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="E1" s="19" t="s">
+      <x:c r="E1" s="17" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="11" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="G1" s="19" t="s">
+      <x:c r="G1" s="17" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="11" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="I1" s="19" t="s">
+      <x:c r="I1" s="17" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="13" t="s">
+      <x:c r="J1" s="11" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:10">
-      <x:c r="A2" s="13" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B2" s="17" t="n">
+      <x:c r="B2" s="15" t="n">
         <x:v>192876928790</x:v>
       </x:c>
-      <x:c r="D2" s="13" t="s"/>
+      <x:c r="D2" s="11" t="s"/>
     </x:row>
     <x:row r="3" spans="1:10">
-      <x:c r="A3" s="13" t="s">
+      <x:c r="A3" s="11" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="B3" s="17" t="n">
+      <x:c r="B3" s="15" t="n">
         <x:v>730143312714</x:v>
       </x:c>
-      <x:c r="D3" s="13" t="s"/>
+      <x:c r="D3" s="11" t="s"/>
     </x:row>
     <x:row r="4" spans="1:10">
-      <x:c r="A4" s="13" t="s">
+      <x:c r="A4" s="11" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B4" s="17" t="n">
+      <x:c r="B4" s="15" t="n">
         <x:v>730143312042</x:v>
       </x:c>
-      <x:c r="D4" s="13" t="s"/>
+      <x:c r="D4" s="11" t="s"/>
     </x:row>
     <x:row r="5" spans="1:10">
-      <x:c r="A5" s="13" t="s">
+      <x:c r="A5" s="11" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="B5" s="17" t="n">
+      <x:c r="B5" s="15" t="n">
         <x:v>735858446006</x:v>
       </x:c>
-      <x:c r="D5" s="13" t="s"/>
+      <x:c r="D5" s="11" t="s"/>
     </x:row>
     <x:row r="6" spans="1:10">
-      <x:c r="A6" s="13" t="s">
+      <x:c r="A6" s="11" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="B6" s="20" t="n">
+      <x:c r="B6" s="18" t="n">
         <x:v>840006604839</x:v>
       </x:c>
-      <x:c r="D6" s="13" t="s"/>
+      <x:c r="D6" s="11" t="s"/>
     </x:row>
     <x:row r="7" spans="1:10">
-      <x:c r="A7" s="13" t="s">
+      <x:c r="A7" s="11" t="s">
         <x:v>64</x:v>
       </x:c>
-      <x:c r="B7" s="21" t="n">
+      <x:c r="B7" s="19" t="n">
         <x:v>824142218600</x:v>
       </x:c>
-      <x:c r="D7" s="13" t="s"/>
+      <x:c r="D7" s="11" t="s"/>
     </x:row>
     <x:row r="8" spans="1:10">
-      <x:c r="A8" s="13" t="s">
+      <x:c r="A8" s="11" t="s">
         <x:v>65</x:v>
       </x:c>
-      <x:c r="B8" s="20" t="n">
+      <x:c r="B8" s="18" t="n">
         <x:v>840006636656</x:v>
       </x:c>
-      <x:c r="D8" s="13" t="s"/>
+      <x:c r="D8" s="11" t="s"/>
     </x:row>
     <x:row r="9" spans="1:10">
-      <x:c r="A9" s="13" t="s">
+      <x:c r="A9" s="11" t="s">
         <x:v>66</x:v>
       </x:c>
-      <x:c r="B9" s="17" t="n">
+      <x:c r="B9" s="15" t="n">
         <x:v>843591058124</x:v>
       </x:c>
-      <x:c r="D9" s="13" t="s"/>
+      <x:c r="D9" s="11" t="s"/>
     </x:row>
     <x:row r="10" spans="1:10">
-      <x:c r="A10" s="13" t="s">
+      <x:c r="A10" s="11" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="B10" s="17" t="n">
+      <x:c r="B10" s="15" t="n">
         <x:v>824142242148</x:v>
       </x:c>
-      <x:c r="D10" s="13" t="s"/>
+      <x:c r="D10" s="11" t="s"/>
     </x:row>
     <x:row r="11" spans="1:10">
-      <x:c r="A11" s="13" t="s">
+      <x:c r="A11" s="11" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="B11" s="17" t="n">
+      <x:c r="B11" s="15" t="n">
         <x:v>840006630609</x:v>
       </x:c>
-      <x:c r="D11" s="13" t="s"/>
+      <x:c r="D11" s="11" t="s"/>
     </x:row>
     <x:row r="12" spans="1:10">
-      <x:c r="A12" s="13" t="s">
+      <x:c r="A12" s="11" t="s">
         <x:v>69</x:v>
       </x:c>
-      <x:c r="B12" s="17" t="n">
+      <x:c r="B12" s="15" t="n">
         <x:v>840006616696</x:v>
       </x:c>
-      <x:c r="D12" s="13" t="s"/>
+      <x:c r="D12" s="11" t="s"/>
     </x:row>
     <x:row r="13" spans="1:10">
-      <x:c r="A13" s="13" t="s">
+      <x:c r="A13" s="11" t="s">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="B13" s="17" t="n">
+      <x:c r="B13" s="15" t="n">
         <x:v>840006627470</x:v>
       </x:c>
-      <x:c r="D13" s="13" t="s"/>
+      <x:c r="D13" s="11" t="s"/>
     </x:row>
     <x:row r="14" spans="1:10">
-      <x:c r="A14" s="13" t="s">
+      <x:c r="A14" s="11" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="B14" s="17" t="n">
+      <x:c r="B14" s="15" t="n">
         <x:v>730143309936</x:v>
       </x:c>
-      <x:c r="D14" s="13" t="s"/>
+      <x:c r="D14" s="11" t="s"/>
     </x:row>
     <x:row r="15" spans="1:10">
-      <x:c r="A15" s="13" t="s">
+      <x:c r="A15" s="11" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="B15" s="17" t="n">
+      <x:c r="B15" s="15" t="n">
         <x:v>889523019023</x:v>
       </x:c>
-      <x:c r="D15" s="13" t="s"/>
+      <x:c r="D15" s="11" t="s"/>
     </x:row>
     <x:row r="16" spans="1:10">
-      <x:c r="A16" s="13" t="s">
+      <x:c r="A16" s="11" t="s">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="B16" s="17" t="n">
+      <x:c r="B16" s="15" t="n">
         <x:v>848354033103</x:v>
       </x:c>
-      <x:c r="D16" s="13" t="s"/>
+      <x:c r="D16" s="11" t="s"/>
     </x:row>
     <x:row r="17" spans="1:10">
-      <x:c r="A17" s="13" t="s">
+      <x:c r="A17" s="11" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="B17" s="17" t="n">
+      <x:c r="B17" s="15" t="n">
         <x:v>718037815367</x:v>
       </x:c>
-      <x:c r="D17" s="13" t="s"/>
+      <x:c r="D17" s="11" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -1344,390 +1472,519 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0300-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:L17"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="L5" sqref="L5 L5:L5"/>
+    <x:sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <x:selection activeCell="H22" sqref="H22 H22:H22"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="13.2"/>
+  <x:sheetFormatPr defaultRowHeight="12.75"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.441406" style="13" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="15.664062" style="13" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="16.554688" style="13" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="16.886719" style="13" customWidth="1"/>
-    <x:col min="5" max="5" width="12.441406" style="13" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="9" width="9.140625" style="13" customWidth="1"/>
-    <x:col min="10" max="10" width="11.554688" style="13" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="15.425781" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="15.710938" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="16.570312" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="16.855469" style="11" customWidth="1"/>
+    <x:col min="5" max="5" width="12.425781" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="7" width="9.140625" style="11" customWidth="1"/>
+    <x:col min="8" max="8" width="169.425781" style="11" bestFit="1" customWidth="1"/>
+    <x:col min="9" max="9" width="9.140625" style="11" customWidth="1"/>
+    <x:col min="10" max="10" width="11.570312" style="11" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:12">
-      <x:c r="A1" s="13" t="s">
+      <x:c r="A1" s="11" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="B1" s="13" t="s">
+      <x:c r="B1" s="11" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="C1" s="13" t="s">
+      <x:c r="C1" s="11" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="D1" s="13" t="s">
+      <x:c r="D1" s="11" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="E1" s="13" t="s">
+      <x:c r="E1" s="11" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="F1" s="13" t="s">
+      <x:c r="F1" s="11" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="G1" s="13" t="s">
+      <x:c r="G1" s="11" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="H1" s="13" t="s">
+      <x:c r="H1" s="11" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="I1" s="13" t="s">
+      <x:c r="I1" s="11" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="13" t="s">
+      <x:c r="J1" s="11" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:12">
-      <x:c r="A2" s="13" t="s">
+      <x:c r="A2" s="11" t="s">
         <x:v>59</x:v>
       </x:c>
-      <x:c r="B2" s="13" t="n">
+      <x:c r="B2" s="11" t="n">
         <x:v>192876928790</x:v>
       </x:c>
-      <x:c r="C2" s="22" t="s"/>
-      <x:c r="D2" s="13" t="s"/>
-      <x:c r="E2" s="13" t="s"/>
-      <x:c r="F2" s="13" t="s"/>
-      <x:c r="G2" s="13" t="s">
+      <x:c r="C2" s="20" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="H2" s="13" t="s">
+      <x:c r="D2" s="11" t="s">
         <x:v>76</x:v>
       </x:c>
-      <x:c r="I2" s="13" t="s"/>
-      <x:c r="J2" s="13" t="s"/>
+      <x:c r="E2" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F2" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G2" s="11" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="H2" s="11" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="I2" s="11" t="s"/>
+      <x:c r="J2" s="11" t="s"/>
     </x:row>
     <x:row r="3" spans="1:12">
-      <x:c r="A3" s="13" t="s">
+      <x:c r="A3" s="11" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="B3" s="13" t="n">
+      <x:c r="B3" s="11" t="n">
         <x:v>730143312714</x:v>
       </x:c>
-      <x:c r="C3" s="22" t="s"/>
-      <x:c r="D3" s="13" t="s"/>
-      <x:c r="E3" s="13" t="s"/>
-      <x:c r="F3" s="13" t="s"/>
-      <x:c r="G3" s="13" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="H3" s="13" t="s">
-        <x:v>78</x:v>
-      </x:c>
-      <x:c r="I3" s="13" t="s"/>
-      <x:c r="J3" s="13" t="s"/>
+      <x:c r="C3" s="20" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="D3" s="11" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="E3" s="11" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="F3" s="11" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="G3" s="11" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="H3" s="11" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="I3" s="11" t="s"/>
+      <x:c r="J3" s="11" t="s"/>
     </x:row>
     <x:row r="4" spans="1:12">
-      <x:c r="A4" s="13" t="s">
+      <x:c r="A4" s="11" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="B4" s="22" t="n">
+      <x:c r="B4" s="20" t="n">
         <x:v>730143312042</x:v>
       </x:c>
-      <x:c r="C4" s="22" t="s"/>
-      <x:c r="D4" s="13" t="s"/>
-      <x:c r="E4" s="13" t="s"/>
-      <x:c r="F4" s="13" t="s"/>
-      <x:c r="G4" s="13" t="s">
-        <x:v>79</x:v>
-      </x:c>
-      <x:c r="H4" s="13" t="s">
-        <x:v>80</x:v>
-      </x:c>
-      <x:c r="I4" s="13" t="s"/>
-      <x:c r="J4" s="13" t="s"/>
+      <x:c r="C4" s="20" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D4" s="11" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="E4" s="11" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="F4" s="11" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="G4" s="11" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="H4" s="11" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="I4" s="11" t="s"/>
+      <x:c r="J4" s="11" t="s"/>
     </x:row>
     <x:row r="5" spans="1:12">
-      <x:c r="A5" s="13" t="s">
+      <x:c r="A5" s="11" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="B5" s="22" t="n">
+      <x:c r="B5" s="20" t="n">
         <x:v>735858446006</x:v>
       </x:c>
-      <x:c r="C5" s="22" t="s"/>
-      <x:c r="D5" s="13" t="s"/>
-      <x:c r="E5" s="13" t="s"/>
-      <x:c r="F5" s="13" t="s"/>
-      <x:c r="G5" s="13" t="s">
-        <x:v>81</x:v>
-      </x:c>
-      <x:c r="H5" s="13" t="s">
-        <x:v>82</x:v>
-      </x:c>
-      <x:c r="I5" s="13" t="s"/>
-      <x:c r="J5" s="13" t="s"/>
-      <x:c r="K5" s="22">
-        <x:f>MIN(C5:G5)</x:f>
-      </x:c>
-      <x:c r="L5" s="13" t="s"/>
+      <x:c r="C5" s="20" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D5" s="11" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="E5" s="11" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="F5" s="11" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="G5" s="11" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="H5" s="11" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="I5" s="11" t="s"/>
+      <x:c r="J5" s="11" t="s"/>
+      <x:c r="K5" s="20" t="s"/>
+      <x:c r="L5" s="11" t="s"/>
     </x:row>
     <x:row r="6" spans="1:12">
-      <x:c r="A6" s="13" t="s">
+      <x:c r="A6" s="11" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="B6" s="22" t="n">
+      <x:c r="B6" s="20" t="n">
         <x:v>840006604839</x:v>
       </x:c>
-      <x:c r="C6" s="22" t="s"/>
-      <x:c r="D6" s="13" t="s"/>
-      <x:c r="E6" s="13" t="s"/>
-      <x:c r="F6" s="13" t="s"/>
-      <x:c r="G6" s="13" t="s">
-        <x:v>83</x:v>
-      </x:c>
-      <x:c r="H6" s="13" t="s">
+      <x:c r="C6" s="20" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D6" s="11" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="E6" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F6" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G6" s="11" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="H6" s="11" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="I6" s="11" t="s"/>
+      <x:c r="J6" s="11" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:12">
+      <x:c r="A7" s="11" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B7" s="20" t="n">
+        <x:v>824142218600</x:v>
+      </x:c>
+      <x:c r="C7" s="20" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="D7" s="11" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E7" s="11" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="F7" s="11" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="G7" s="11" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="H7" s="11" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="I7" s="11" t="s"/>
+      <x:c r="J7" s="11" t="s"/>
+      <x:c r="K7" s="20" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:12">
+      <x:c r="A8" s="11" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B8" s="20" t="n">
+        <x:v>840006636656</x:v>
+      </x:c>
+      <x:c r="C8" s="20" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="D8" s="11" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="E8" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F8" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G8" s="11" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="H8" s="11" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="I8" s="11" t="s"/>
+      <x:c r="J8" s="11" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:12">
+      <x:c r="A9" s="11" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B9" s="20" t="n">
+        <x:v>843591058124</x:v>
+      </x:c>
+      <x:c r="C9" s="20" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="D9" s="11" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="E9" s="11" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="F9" s="11" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="G9" s="11" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="H9" s="11" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="I9" s="11" t="s"/>
+      <x:c r="J9" s="11" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:12">
+      <x:c r="A10" s="11" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B10" s="20" t="n">
+        <x:v>824142242148</x:v>
+      </x:c>
+      <x:c r="C10" s="20" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="D10" s="11" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="E10" s="11" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="F10" s="11" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="G10" s="11" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="H10" s="11" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="I10" s="11" t="s"/>
+      <x:c r="J10" s="11" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:12">
+      <x:c r="A11" s="11" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B11" s="20" t="n">
+        <x:v>840006630609</x:v>
+      </x:c>
+      <x:c r="C11" s="20" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="D11" s="11" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="E11" s="11" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="F11" s="11" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="G11" s="11" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="H11" s="11" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="I11" s="11" t="s"/>
+      <x:c r="J11" s="11" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:12">
+      <x:c r="A12" s="11" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B12" s="20" t="n">
+        <x:v>840006616696</x:v>
+      </x:c>
+      <x:c r="C12" s="20" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="D12" s="11" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="E12" s="11" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="F12" s="11" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="G12" s="11" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="H12" s="11" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="I12" s="11" t="s"/>
+      <x:c r="J12" s="11" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:12">
+      <x:c r="A13" s="11" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B13" s="20" t="n">
+        <x:v>840006627470</x:v>
+      </x:c>
+      <x:c r="C13" s="20" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="D13" s="11" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="E13" s="11" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="F13" s="11" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G13" s="11" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="H13" s="11" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="I13" s="11" t="s"/>
+      <x:c r="J13" s="11" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:12">
+      <x:c r="A14" s="11" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B14" s="20" t="n">
+        <x:v>730143309936</x:v>
+      </x:c>
+      <x:c r="C14" s="20" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="D14" s="11" t="s">
+        <x:v>132</x:v>
+      </x:c>
+      <x:c r="E14" s="11" t="s">
+        <x:v>131</x:v>
+      </x:c>
+      <x:c r="F14" s="11" t="s">
+        <x:v>133</x:v>
+      </x:c>
+      <x:c r="G14" s="11" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="H14" s="11" t="s">
         <x:v>84</x:v>
       </x:c>
-      <x:c r="I6" s="13" t="s"/>
-      <x:c r="J6" s="13" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:12">
-      <x:c r="A7" s="13" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="B7" s="22" t="n">
-        <x:v>824142218600</x:v>
-      </x:c>
-      <x:c r="C7" s="22" t="s"/>
-      <x:c r="D7" s="13" t="s"/>
-      <x:c r="E7" s="13" t="s"/>
-      <x:c r="F7" s="13" t="s"/>
-      <x:c r="G7" s="13" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="H7" s="13" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="I7" s="13" t="s"/>
-      <x:c r="J7" s="13" t="s"/>
-      <x:c r="K7" s="22">
-        <x:f>MIN(C7:G7)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:12">
-      <x:c r="A8" s="13" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="B8" s="22" t="n">
-        <x:v>840006636656</x:v>
-      </x:c>
-      <x:c r="C8" s="22" t="s"/>
-      <x:c r="D8" s="13" t="s"/>
-      <x:c r="E8" s="13" t="s"/>
-      <x:c r="F8" s="13" t="s"/>
-      <x:c r="G8" s="13" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="H8" s="13" t="s">
-        <x:v>88</x:v>
-      </x:c>
-      <x:c r="I8" s="13" t="s"/>
-      <x:c r="J8" s="13" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:12">
-      <x:c r="A9" s="13" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="B9" s="22" t="n">
-        <x:v>843591058124</x:v>
-      </x:c>
-      <x:c r="C9" s="22" t="s"/>
-      <x:c r="D9" s="13" t="s"/>
-      <x:c r="E9" s="13" t="s"/>
-      <x:c r="F9" s="13" t="s"/>
-      <x:c r="G9" s="13" t="s">
-        <x:v>89</x:v>
-      </x:c>
-      <x:c r="H9" s="13" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="I9" s="13" t="s"/>
-      <x:c r="J9" s="13" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:12">
-      <x:c r="A10" s="13" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="B10" s="22" t="n">
-        <x:v>824142242148</x:v>
-      </x:c>
-      <x:c r="C10" s="22" t="s"/>
-      <x:c r="D10" s="13" t="s"/>
-      <x:c r="E10" s="13" t="s"/>
-      <x:c r="F10" s="13" t="s"/>
-      <x:c r="G10" s="13" t="s">
+      <x:c r="I14" s="11" t="s"/>
+      <x:c r="J14" s="11" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:12">
+      <x:c r="A15" s="11" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B15" s="20" t="n">
+        <x:v>889523019023</x:v>
+      </x:c>
+      <x:c r="C15" s="20" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D15" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E15" s="11" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="F15" s="11" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="G15" s="11" t="s">
+        <x:v>136</x:v>
+      </x:c>
+      <x:c r="H15" s="11" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="I15" s="11" t="s"/>
+      <x:c r="J15" s="11" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:12">
+      <x:c r="A16" s="11" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B16" s="20" t="n">
+        <x:v>848354033103</x:v>
+      </x:c>
+      <x:c r="C16" s="20" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D16" s="11" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E16" s="11" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="F16" s="11" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="G16" s="11" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="H10" s="13" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="I10" s="13" t="s"/>
-      <x:c r="J10" s="13" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:12">
-      <x:c r="A11" s="13" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="B11" s="22" t="n">
-        <x:v>840006630609</x:v>
-      </x:c>
-      <x:c r="C11" s="22" t="s"/>
-      <x:c r="D11" s="13" t="s"/>
-      <x:c r="E11" s="13" t="s"/>
-      <x:c r="F11" s="13" t="s"/>
-      <x:c r="G11" s="13" t="s">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="H11" s="13" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="I11" s="13" t="s"/>
-      <x:c r="J11" s="13" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:12">
-      <x:c r="A12" s="13" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="B12" s="22" t="n">
-        <x:v>840006616696</x:v>
-      </x:c>
-      <x:c r="C12" s="22" t="s"/>
-      <x:c r="D12" s="13" t="s"/>
-      <x:c r="E12" s="13" t="s"/>
-      <x:c r="F12" s="13" t="s"/>
-      <x:c r="G12" s="13" t="s">
-        <x:v>85</x:v>
-      </x:c>
-      <x:c r="H12" s="13" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="I12" s="13" t="s"/>
-      <x:c r="J12" s="13" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:12">
-      <x:c r="A13" s="13" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="B13" s="22" t="n">
-        <x:v>840006627470</x:v>
-      </x:c>
-      <x:c r="C13" s="22" t="s"/>
-      <x:c r="D13" s="13" t="s"/>
-      <x:c r="E13" s="13" t="s"/>
-      <x:c r="F13" s="13" t="s"/>
-      <x:c r="G13" s="13" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="H13" s="13" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="I13" s="13" t="s"/>
-      <x:c r="J13" s="13" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:12">
-      <x:c r="A14" s="13" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="B14" s="22" t="n">
-        <x:v>730143309936</x:v>
-      </x:c>
-      <x:c r="C14" s="22" t="s"/>
-      <x:c r="D14" s="13" t="s"/>
-      <x:c r="E14" s="13" t="s"/>
-      <x:c r="F14" s="13" t="s"/>
-      <x:c r="G14" s="13" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="H14" s="13" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="I14" s="13" t="s"/>
-      <x:c r="J14" s="13" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:12">
-      <x:c r="A15" s="13" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="B15" s="22" t="n">
-        <x:v>889523019023</x:v>
-      </x:c>
-      <x:c r="C15" s="22" t="s"/>
-      <x:c r="D15" s="13" t="s"/>
-      <x:c r="E15" s="13" t="s"/>
-      <x:c r="F15" s="13" t="s"/>
-      <x:c r="G15" s="13" t="s">
-        <x:v>100</x:v>
-      </x:c>
-      <x:c r="H15" s="13" t="s">
-        <x:v>101</x:v>
-      </x:c>
-      <x:c r="I15" s="13" t="s"/>
-      <x:c r="J15" s="13" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:12">
-      <x:c r="A16" s="13" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="B16" s="22" t="n">
-        <x:v>848354033103</x:v>
-      </x:c>
-      <x:c r="C16" s="22" t="s"/>
-      <x:c r="D16" s="13" t="s"/>
-      <x:c r="E16" s="13" t="s"/>
-      <x:c r="F16" s="13" t="s"/>
-      <x:c r="G16" s="13" t="s">
-        <x:v>96</x:v>
-      </x:c>
-      <x:c r="H16" s="13" t="s">
-        <x:v>102</x:v>
-      </x:c>
-      <x:c r="I16" s="13" t="s"/>
-      <x:c r="J16" s="13" t="s"/>
+      <x:c r="H16" s="11" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="I16" s="11" t="s"/>
+      <x:c r="J16" s="11" t="s"/>
     </x:row>
     <x:row r="17" spans="1:12">
-      <x:c r="A17" s="13" t="s">
+      <x:c r="A17" s="11" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="B17" s="22" t="n">
+      <x:c r="B17" s="20" t="n">
         <x:v>718037815367</x:v>
       </x:c>
-      <x:c r="C17" s="22" t="s"/>
-      <x:c r="D17" s="13" t="s"/>
-      <x:c r="E17" s="13" t="s"/>
-      <x:c r="F17" s="13" t="s"/>
-      <x:c r="G17" s="13" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="H17" s="13" t="s">
-        <x:v>104</x:v>
-      </x:c>
-      <x:c r="I17" s="13" t="s"/>
-      <x:c r="J17" s="13" t="s"/>
+      <x:c r="C17" s="20" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="D17" s="11" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="E17" s="11" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="F17" s="11" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="G17" s="11" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="H17" s="11" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="I17" s="11" t="s"/>
+      <x:c r="J17" s="11" t="s"/>
+    </x:row>
+    <x:row r="22" spans="1:12">
+      <x:c r="H22" s="11" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>